<commit_message>
add values to input_output excel
</commit_message>
<xml_diff>
--- a/excel_tax_calculation/input_output/input_output.xlsx
+++ b/excel_tax_calculation/input_output/input_output.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/benjamin.van.dam/Documents/codebases/be_market/excel_tax_calculation/input_output/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annelot.audenaert/Documents/be_market/excel_tax_calculation/input_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5AAF252-7629-3A48-84E2-E60DFE713CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6485E3C3-39E3-5748-9C60-CB53FC45B4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{B5C74626-8E96-454A-A0EA-D4ED5FC94566}"/>
+    <workbookView xWindow="36300" yWindow="2620" windowWidth="28040" windowHeight="16280" xr2:uid="{B5C74626-8E96-454A-A0EA-D4ED5FC94566}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Results" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>Input</t>
   </si>
@@ -50,9 +50,6 @@
     <t>Version Calculation Excel</t>
   </si>
   <si>
-    <t>v0</t>
-  </si>
-  <si>
     <t>tax_calc_no_glob</t>
   </si>
   <si>
@@ -63,6 +60,18 @@
   </si>
   <si>
     <t>tax_calc_glob_p1_p2</t>
+  </si>
+  <si>
+    <t>solde glob 0</t>
+  </si>
+  <si>
+    <t>solde p1</t>
+  </si>
+  <si>
+    <t>solde p2</t>
+  </si>
+  <si>
+    <t>solde p1_p2</t>
   </si>
 </sst>
 </file>
@@ -110,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -121,6 +130,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,21 +465,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D0DD7E5-79A9-5C4D-8B9F-F15347AA3655}">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="14.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.1640625" customWidth="1"/>
+    <col min="6" max="6" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.1640625" customWidth="1"/>
+    <col min="8" max="8" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.1640625" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C1" s="3" t="s">
         <v>1</v>
       </c>
@@ -477,8 +493,11 @@
       <c r="E1" s="3"/>
       <c r="F1" s="3"/>
       <c r="G1" s="3"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
+      <c r="J1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -489,29 +508,62 @@
         <v>2</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="G2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="I2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="G2" s="2" t="s">
-        <v>8</v>
+      <c r="K2" s="1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>79122109350</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
+      <c r="D3" s="4">
+        <v>-16207.56</v>
+      </c>
+      <c r="E3">
+        <v>-1357.34</v>
+      </c>
+      <c r="F3" s="4">
+        <v>-16168.27</v>
+      </c>
+      <c r="G3">
+        <v>-1318.26</v>
+      </c>
+      <c r="H3">
+        <v>-16207.56</v>
+      </c>
+      <c r="I3">
+        <v>-1357.34</v>
+      </c>
+      <c r="J3">
+        <v>-16168.27</v>
+      </c>
+      <c r="K3">
+        <v>-1318.26</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="C1:G1"/>
+    <mergeCell ref="C1:J1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
add solde values in input_output and filled in original big case
</commit_message>
<xml_diff>
--- a/excel_tax_calculation/input_output/input_output.xlsx
+++ b/excel_tax_calculation/input_output/input_output.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/annelot.audenaert/Documents/be_market/excel_tax_calculation/input_output/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6485E3C3-39E3-5748-9C60-CB53FC45B4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63FC1B5D-1647-9345-8688-A4D2128F51BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="36300" yWindow="2620" windowWidth="28040" windowHeight="16280" xr2:uid="{B5C74626-8E96-454A-A0EA-D4ED5FC94566}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>Input</t>
   </si>
@@ -72,6 +72,9 @@
   </si>
   <si>
     <t>solde p1_p2</t>
+  </si>
+  <si>
+    <t>version 1 for no glob and p1, version 2 for p2 and p1_P2</t>
   </si>
 </sst>
 </file>
@@ -127,10 +130,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,7 +471,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -486,16 +489,16 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
@@ -536,13 +539,16 @@
       <c r="A3">
         <v>79122109350</v>
       </c>
-      <c r="D3" s="4">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="3">
         <v>-16207.56</v>
       </c>
       <c r="E3">
         <v>-1357.34</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>-16168.27</v>
       </c>
       <c r="G3">

</xml_diff>